<commit_message>
Tree Proxy validation set
</commit_message>
<xml_diff>
--- a/Prototypes/Agroforestry/Observed.xlsx
+++ b/Prototypes/Agroforestry/Observed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="18">
   <si>
     <t>SimulationName</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>GrainWt</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>GrainSize</t>
+  </si>
+  <si>
+    <t>GrainNumber</t>
   </si>
 </sst>
 </file>
@@ -393,20 +402,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,1484 +423,1847 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
         <v>38068</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>246.2748</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
         <v>38135</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>228.3006</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
         <v>38212</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>181.70580000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
         <v>38247</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>169.43270000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
         <v>38278</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>170.18610000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
         <v>38315</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>172.2295</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
         <v>38336</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>163.44290000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
         <v>38365</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>156.7268</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
         <v>38393</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>159.3176</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
         <v>38426</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>156.60409999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
         <v>38562</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>217.93289999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
         <v>38629</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>175.5197</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
         <v>38068</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>265.44130000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
         <v>38135</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>233.82040000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
         <v>38212</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>203.32509999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
         <v>38247</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>186.1858</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>1</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
         <v>38278</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>224.417</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
         <v>38286</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>1</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
         <v>38315</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>218.7561</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>1</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
         <v>38336</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>211.67570000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>1</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1">
         <v>38365</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>196.32560000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1">
         <v>38393</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>196.7028</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>1</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1">
         <v>38426</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>187.02440000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
         <v>38562</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>231.30699999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>1</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1">
         <v>38629</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>184.66589999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>1</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1">
         <v>38068</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>280.70209999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>1</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1">
         <v>38135</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>247.74449999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1">
         <v>38212</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>208.29060000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1">
         <v>38247</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>189.74270000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>1</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1">
         <v>38278</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>221.0035</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>1</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1">
         <v>38286</v>
       </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1">
         <v>38315</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>227.10910000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>1</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1">
         <v>38336</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>218.99539999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>1</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1">
         <v>38365</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>207.06899999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1">
         <v>38393</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>204.21860000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>1</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37" s="1">
         <v>38426</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>197.74440000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>1</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38" s="1">
         <v>38562</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>245.0915</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>1</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1">
         <v>38629</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>193.00380000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>1</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40">
+        <v>15</v>
+      </c>
+      <c r="D40" s="1">
         <v>38068</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>315.4982</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>1</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41">
+        <v>15</v>
+      </c>
+      <c r="D41" s="1">
         <v>38135</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>294.81180000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>1</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42">
+        <v>15</v>
+      </c>
+      <c r="D42" s="1">
         <v>38212</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>220.4307</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>1</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43">
+        <v>15</v>
+      </c>
+      <c r="D43" s="1">
         <v>38247</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>194.06720000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>1</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44">
+        <v>15</v>
+      </c>
+      <c r="D44" s="1">
         <v>38278</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>231.0966</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>1</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45">
+        <v>15</v>
+      </c>
+      <c r="D45" s="1">
         <v>38286</v>
       </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
       <c r="F45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>1</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46">
+        <v>15</v>
+      </c>
+      <c r="D46" s="1">
         <v>38315</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>244.6534</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>1</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47">
+        <v>15</v>
+      </c>
+      <c r="D47" s="1">
         <v>38336</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>246.68809999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>1</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48">
+        <v>15</v>
+      </c>
+      <c r="D48" s="1">
         <v>38365</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>226.98060000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>1</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49">
+        <v>15</v>
+      </c>
+      <c r="D49" s="1">
         <v>38393</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>227.02959999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>1</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50">
+        <v>15</v>
+      </c>
+      <c r="D50" s="1">
         <v>38426</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>217.83080000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>1</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51">
+        <v>15</v>
+      </c>
+      <c r="D51" s="1">
         <v>38562</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>279.34480000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>1</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52">
+        <v>15</v>
+      </c>
+      <c r="D52" s="1">
         <v>38629</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>226.07589999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>1</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53">
+        <v>20</v>
+      </c>
+      <c r="D53" s="1">
         <v>38068</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>329.68729999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>1</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54">
+        <v>20</v>
+      </c>
+      <c r="D54" s="1">
         <v>38135</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>326.65600000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>1</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55">
+        <v>20</v>
+      </c>
+      <c r="D55" s="1">
         <v>38212</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>259.3116</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>1</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56">
+        <v>20</v>
+      </c>
+      <c r="D56" s="1">
         <v>38247</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>222.68539999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>1</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57">
+        <v>20</v>
+      </c>
+      <c r="D57" s="1">
         <v>38278</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>257.69330000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>1</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58">
+        <v>20</v>
+      </c>
+      <c r="D58" s="1">
         <v>38286</v>
       </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>1</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59">
+        <v>20</v>
+      </c>
+      <c r="D59" s="1">
         <v>38315</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>276.83370000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>1</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60">
+        <v>20</v>
+      </c>
+      <c r="D60" s="1">
         <v>38336</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>292.7987</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>1</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61">
+        <v>20</v>
+      </c>
+      <c r="D61" s="1">
         <v>38365</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>280.30110000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>1</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62" s="1">
         <v>38393</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>291.54480000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>1</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63">
+        <v>20</v>
+      </c>
+      <c r="D63" s="1">
         <v>38426</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>274.55829999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>1</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64">
+        <v>20</v>
+      </c>
+      <c r="D64" s="1">
         <v>38562</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>311.77859999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>1</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65">
+        <v>20</v>
+      </c>
+      <c r="D65" s="1">
         <v>38629</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>270.01639999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>1</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66">
+        <v>30</v>
+      </c>
+      <c r="D66" s="1">
         <v>38068</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>326.52960000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>1</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67">
+        <v>30</v>
+      </c>
+      <c r="D67" s="1">
         <v>38135</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>322.03030000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>1</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68">
+        <v>30</v>
+      </c>
+      <c r="D68" s="1">
         <v>38212</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>278.7346</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>1</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69">
+        <v>30</v>
+      </c>
+      <c r="D69" s="1">
         <v>38247</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>238.69569999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>1</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70">
+        <v>30</v>
+      </c>
+      <c r="D70" s="1">
         <v>38278</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>240.60050000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>1</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71">
+        <v>30</v>
+      </c>
+      <c r="D71" s="1">
         <v>38286</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>470.36250000000001</v>
       </c>
-      <c r="F71">
+      <c r="G71">
         <v>190.334475</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="H71">
+        <v>2.4674999999999999E-2</v>
+      </c>
+      <c r="I71">
+        <f>G71/H71</f>
+        <v>7713.6565349544071</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>1</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72">
+        <v>30</v>
+      </c>
+      <c r="D72" s="1">
         <v>38315</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>290.78410000000002</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>1</v>
       </c>
       <c r="B73" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73">
+        <v>30</v>
+      </c>
+      <c r="D73" s="1">
         <v>38336</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>285.52730000000003</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>1</v>
       </c>
       <c r="B74" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74">
+        <v>30</v>
+      </c>
+      <c r="D74" s="1">
         <v>38365</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>285.9622</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>1</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75">
+        <v>30</v>
+      </c>
+      <c r="D75" s="1">
         <v>38393</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>299.47840000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>1</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76">
+        <v>30</v>
+      </c>
+      <c r="D76" s="1">
         <v>38426</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>305.68150000000003</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>1</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77">
+        <v>30</v>
+      </c>
+      <c r="D77" s="1">
         <v>38562</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>329.28820000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>1</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78">
+        <v>30</v>
+      </c>
+      <c r="D78" s="1">
         <v>38629</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>306.47559999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>1</v>
       </c>
       <c r="B79" t="s">
         <v>10</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79">
+        <v>40</v>
+      </c>
+      <c r="D79" s="1">
         <v>38068</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <v>311.55110000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>1</v>
       </c>
       <c r="B80" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80">
+        <v>40</v>
+      </c>
+      <c r="D80" s="1">
         <v>38135</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>312.97140000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>1</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81">
+        <v>40</v>
+      </c>
+      <c r="D81" s="1">
         <v>38212</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>265.67770000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>1</v>
       </c>
       <c r="B82" t="s">
         <v>10</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82">
+        <v>40</v>
+      </c>
+      <c r="D82" s="1">
         <v>38247</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>225.32929999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>1</v>
       </c>
       <c r="B83" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83">
+        <v>40</v>
+      </c>
+      <c r="D83" s="1">
         <v>38278</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>219.2167</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>1</v>
       </c>
       <c r="B84" t="s">
         <v>10</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84">
+        <v>40</v>
+      </c>
+      <c r="D84" s="1">
         <v>38286</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>823.84199999999998</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>339.20711999999997</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="H84">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I84">
+        <f>G84/H84</f>
+        <v>11696.797241379309</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>1</v>
       </c>
       <c r="B85" t="s">
         <v>10</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85">
+        <v>40</v>
+      </c>
+      <c r="D85" s="1">
         <v>38315</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>271.93110000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>1</v>
       </c>
       <c r="B86" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86">
+        <v>40</v>
+      </c>
+      <c r="D86" s="1">
         <v>38336</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <v>272.42020000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>1</v>
       </c>
       <c r="B87" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87">
+        <v>40</v>
+      </c>
+      <c r="D87" s="1">
         <v>38365</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>277.8494</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>1</v>
       </c>
       <c r="B88" t="s">
         <v>10</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88">
+        <v>40</v>
+      </c>
+      <c r="D88" s="1">
         <v>38393</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>282.3415</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>1</v>
       </c>
       <c r="B89" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89">
+        <v>40</v>
+      </c>
+      <c r="D89" s="1">
         <v>38426</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>282.9323</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>1</v>
       </c>
       <c r="B90" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90">
+        <v>40</v>
+      </c>
+      <c r="D90" s="1">
         <v>38562</v>
       </c>
-      <c r="D90">
+      <c r="E90">
         <v>323.94600000000003</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>1</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91">
+        <v>40</v>
+      </c>
+      <c r="D91" s="1">
         <v>38629</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <v>304.19</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>1</v>
       </c>
       <c r="B92" t="s">
         <v>11</v>
       </c>
-      <c r="C92" s="1">
+      <c r="C92">
+        <v>50</v>
+      </c>
+      <c r="D92" s="1">
         <v>38068</v>
       </c>
-      <c r="D92">
+      <c r="E92">
         <v>307.10149999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>1</v>
       </c>
       <c r="B93" t="s">
         <v>11</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C93">
+        <v>50</v>
+      </c>
+      <c r="D93" s="1">
         <v>38135</v>
       </c>
-      <c r="D93">
+      <c r="E93">
         <v>314.42110000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>1</v>
       </c>
       <c r="B94" t="s">
         <v>11</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94">
+        <v>50</v>
+      </c>
+      <c r="D94" s="1">
         <v>38212</v>
       </c>
-      <c r="D94">
+      <c r="E94">
         <v>269.50049999999999</v>
       </c>
-      <c r="E94">
+      <c r="F94">
         <v>206.12700000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>1</v>
       </c>
       <c r="B95" t="s">
         <v>11</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95">
+        <v>50</v>
+      </c>
+      <c r="D95" s="1">
         <v>38247</v>
       </c>
-      <c r="D95">
+      <c r="E95">
         <v>233.7227</v>
       </c>
-      <c r="E95">
+      <c r="F95">
         <v>509.70142857142798</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>1</v>
       </c>
       <c r="B96" t="s">
         <v>11</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96">
+        <v>50</v>
+      </c>
+      <c r="D96" s="1">
         <v>38278</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>218.3073</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>1</v>
       </c>
       <c r="B97" t="s">
         <v>11</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97">
+        <v>50</v>
+      </c>
+      <c r="D97" s="1">
         <v>38286</v>
       </c>
-      <c r="E97">
+      <c r="F97">
         <v>759.24</v>
       </c>
-      <c r="F97">
+      <c r="G97">
         <v>297.93509999999998</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="H97">
+        <v>2.5866699999999999E-2</v>
+      </c>
+      <c r="I97">
+        <f>G97/H97</f>
+        <v>11518.094693176941</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>1</v>
       </c>
       <c r="B98" t="s">
         <v>11</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98">
+        <v>50</v>
+      </c>
+      <c r="D98" s="1">
         <v>38315</v>
       </c>
-      <c r="D98">
+      <c r="E98">
         <v>267.8297</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>1</v>
       </c>
       <c r="B99" t="s">
         <v>11</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99">
+        <v>50</v>
+      </c>
+      <c r="D99" s="1">
         <v>38336</v>
       </c>
-      <c r="D99">
+      <c r="E99">
         <v>279.68970000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>1</v>
       </c>
       <c r="B100" t="s">
         <v>11</v>
       </c>
-      <c r="C100" s="1">
+      <c r="C100">
+        <v>50</v>
+      </c>
+      <c r="D100" s="1">
         <v>38365</v>
       </c>
-      <c r="D100">
+      <c r="E100">
         <v>272.70119999999997</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>1</v>
       </c>
       <c r="B101" t="s">
         <v>11</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101">
+        <v>50</v>
+      </c>
+      <c r="D101" s="1">
         <v>38393</v>
       </c>
-      <c r="D101">
+      <c r="E101">
         <v>299.42110000000002</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>1</v>
       </c>
       <c r="B102" t="s">
         <v>11</v>
       </c>
-      <c r="C102" s="1">
+      <c r="C102">
+        <v>50</v>
+      </c>
+      <c r="D102" s="1">
         <v>38426</v>
       </c>
-      <c r="D102">
+      <c r="E102">
         <v>298.7124</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>1</v>
       </c>
       <c r="B103" t="s">
         <v>11</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C103">
+        <v>50</v>
+      </c>
+      <c r="D103" s="1">
         <v>38562</v>
       </c>
-      <c r="D103">
+      <c r="E103">
         <v>328.44279999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>1</v>
       </c>
       <c r="B104" t="s">
         <v>11</v>
       </c>
-      <c r="C104" s="1">
+      <c r="C104">
+        <v>50</v>
+      </c>
+      <c r="D104" s="1">
         <v>38629</v>
       </c>
-      <c r="D104">
+      <c r="E104">
         <v>306.70319999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor graph code to make more generic and zone aware
</commit_message>
<xml_diff>
--- a/Prototypes/Agroforestry/Observed.xlsx
+++ b/Prototypes/Agroforestry/Observed.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedWarraBlock1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="MooraET" sheetId="3" r:id="rId3"/>
     <sheet name="MooraBiomass" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -20,9 +20,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="29">
   <si>
     <t>SimulationName</t>
-  </si>
-  <si>
-    <t>ZoneName</t>
   </si>
   <si>
     <t>TreeRow</t>
@@ -105,12 +102,15 @@
   <si>
     <t>AboveGround_kg</t>
   </si>
+  <si>
+    <t>Zone</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +148,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -194,7 +202,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,9 +234,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,6 +286,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,55 +479,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -495,12 +539,12 @@
         <v>246.2748</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -512,12 +556,12 @@
         <v>228.3006</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -529,12 +573,12 @@
         <v>181.70580000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -546,12 +590,12 @@
         <v>169.43270000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -563,12 +607,12 @@
         <v>170.18610000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -580,12 +624,12 @@
         <v>172.2295</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -597,12 +641,12 @@
         <v>163.44290000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -614,12 +658,12 @@
         <v>156.7268</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -631,12 +675,12 @@
         <v>159.3176</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -648,12 +692,12 @@
         <v>156.60409999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -665,12 +709,12 @@
         <v>217.93289999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -682,12 +726,12 @@
         <v>175.5197</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -699,12 +743,12 @@
         <v>265.44130000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -716,12 +760,12 @@
         <v>233.82040000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -733,12 +777,12 @@
         <v>203.32509999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -750,12 +794,12 @@
         <v>186.1858</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -767,12 +811,12 @@
         <v>224.417</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -793,12 +837,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -810,12 +854,12 @@
         <v>218.7561</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -827,12 +871,12 @@
         <v>211.67570000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -844,12 +888,12 @@
         <v>196.32560000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -861,12 +905,12 @@
         <v>196.7028</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -878,12 +922,12 @@
         <v>187.02440000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -895,12 +939,12 @@
         <v>231.30699999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -912,12 +956,12 @@
         <v>184.66589999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -929,12 +973,12 @@
         <v>280.70209999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -946,12 +990,12 @@
         <v>247.74449999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -963,12 +1007,12 @@
         <v>208.29060000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30">
         <v>10</v>
@@ -980,12 +1024,12 @@
         <v>189.74270000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -997,12 +1041,12 @@
         <v>221.0035</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -1023,12 +1067,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -1040,12 +1084,12 @@
         <v>227.10910000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34">
         <v>10</v>
@@ -1057,12 +1101,12 @@
         <v>218.99539999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>10</v>
@@ -1074,12 +1118,12 @@
         <v>207.06899999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <v>10</v>
@@ -1091,12 +1135,12 @@
         <v>204.21860000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -1108,12 +1152,12 @@
         <v>197.74440000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -1125,12 +1169,12 @@
         <v>245.0915</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -1142,12 +1186,12 @@
         <v>193.00380000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>15</v>
@@ -1159,12 +1203,12 @@
         <v>315.4982</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>15</v>
@@ -1176,12 +1220,12 @@
         <v>294.81180000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>15</v>
@@ -1193,12 +1237,12 @@
         <v>220.4307</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>15</v>
@@ -1210,12 +1254,12 @@
         <v>194.06720000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>15</v>
@@ -1227,12 +1271,12 @@
         <v>231.0966</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45">
         <v>15</v>
@@ -1253,12 +1297,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46">
         <v>15</v>
@@ -1270,12 +1314,12 @@
         <v>244.6534</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C47">
         <v>15</v>
@@ -1287,12 +1331,12 @@
         <v>246.68809999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48">
         <v>15</v>
@@ -1304,12 +1348,12 @@
         <v>226.98060000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49">
         <v>15</v>
@@ -1321,12 +1365,12 @@
         <v>227.02959999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>15</v>
@@ -1338,12 +1382,12 @@
         <v>217.83080000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51">
         <v>15</v>
@@ -1355,12 +1399,12 @@
         <v>279.34480000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C52">
         <v>15</v>
@@ -1372,12 +1416,12 @@
         <v>226.07589999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53">
         <v>20</v>
@@ -1389,12 +1433,12 @@
         <v>329.68729999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54">
         <v>20</v>
@@ -1406,12 +1450,12 @@
         <v>326.65600000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <v>20</v>
@@ -1423,12 +1467,12 @@
         <v>259.3116</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56">
         <v>20</v>
@@ -1440,12 +1484,12 @@
         <v>222.68539999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57">
         <v>20</v>
@@ -1457,12 +1501,12 @@
         <v>257.69330000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58">
         <v>20</v>
@@ -1483,12 +1527,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C59">
         <v>20</v>
@@ -1500,12 +1544,12 @@
         <v>276.83370000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60">
         <v>20</v>
@@ -1517,12 +1561,12 @@
         <v>292.7987</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61">
         <v>20</v>
@@ -1534,12 +1578,12 @@
         <v>280.30110000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62">
         <v>20</v>
@@ -1551,12 +1595,12 @@
         <v>291.54480000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>20</v>
@@ -1568,12 +1612,12 @@
         <v>274.55829999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <v>20</v>
@@ -1585,12 +1629,12 @@
         <v>311.77859999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>20</v>
@@ -1602,12 +1646,12 @@
         <v>270.01639999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C66">
         <v>30</v>
@@ -1619,12 +1663,12 @@
         <v>326.52960000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C67">
         <v>30</v>
@@ -1636,12 +1680,12 @@
         <v>322.03030000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68">
         <v>30</v>
@@ -1653,12 +1697,12 @@
         <v>278.7346</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C69">
         <v>30</v>
@@ -1670,12 +1714,12 @@
         <v>238.69569999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C70">
         <v>30</v>
@@ -1687,12 +1731,12 @@
         <v>240.60050000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C71">
         <v>30</v>
@@ -1714,12 +1758,12 @@
         <v>7713.6565349544071</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C72">
         <v>30</v>
@@ -1731,12 +1775,12 @@
         <v>290.78410000000002</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C73">
         <v>30</v>
@@ -1748,12 +1792,12 @@
         <v>285.52730000000003</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C74">
         <v>30</v>
@@ -1765,12 +1809,12 @@
         <v>285.9622</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C75">
         <v>30</v>
@@ -1782,12 +1826,12 @@
         <v>299.47840000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C76">
         <v>30</v>
@@ -1799,12 +1843,12 @@
         <v>305.68150000000003</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77">
         <v>30</v>
@@ -1816,12 +1860,12 @@
         <v>329.28820000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C78">
         <v>30</v>
@@ -1833,12 +1877,12 @@
         <v>306.47559999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C79">
         <v>40</v>
@@ -1850,12 +1894,12 @@
         <v>311.55110000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C80">
         <v>40</v>
@@ -1867,12 +1911,12 @@
         <v>312.97140000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C81">
         <v>40</v>
@@ -1884,12 +1928,12 @@
         <v>265.67770000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C82">
         <v>40</v>
@@ -1901,12 +1945,12 @@
         <v>225.32929999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C83">
         <v>40</v>
@@ -1918,12 +1962,12 @@
         <v>219.2167</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C84">
         <v>40</v>
@@ -1945,12 +1989,12 @@
         <v>11696.797241379309</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C85">
         <v>40</v>
@@ -1962,12 +2006,12 @@
         <v>271.93110000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C86">
         <v>40</v>
@@ -1979,12 +2023,12 @@
         <v>272.42020000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C87">
         <v>40</v>
@@ -1996,12 +2040,12 @@
         <v>277.8494</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C88">
         <v>40</v>
@@ -2013,12 +2057,12 @@
         <v>282.3415</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C89">
         <v>40</v>
@@ -2030,12 +2074,12 @@
         <v>282.9323</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B90" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C90">
         <v>40</v>
@@ -2047,12 +2091,12 @@
         <v>323.94600000000003</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C91">
         <v>40</v>
@@ -2064,12 +2108,12 @@
         <v>304.19</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C92">
         <v>50</v>
@@ -2081,12 +2125,12 @@
         <v>307.10149999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C93">
         <v>50</v>
@@ -2098,12 +2142,12 @@
         <v>314.42110000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C94">
         <v>50</v>
@@ -2118,12 +2162,12 @@
         <v>206.12700000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C95">
         <v>50</v>
@@ -2138,12 +2182,12 @@
         <v>509.70142857142798</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C96">
         <v>50</v>
@@ -2155,12 +2199,12 @@
         <v>218.3073</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C97">
         <v>50</v>
@@ -2182,12 +2226,12 @@
         <v>11518.094693176941</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C98">
         <v>50</v>
@@ -2199,12 +2243,12 @@
         <v>267.8297</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C99">
         <v>50</v>
@@ -2216,12 +2260,12 @@
         <v>279.68970000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C100">
         <v>50</v>
@@ -2233,12 +2277,12 @@
         <v>272.70119999999997</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C101">
         <v>50</v>
@@ -2250,12 +2294,12 @@
         <v>299.42110000000002</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C102">
         <v>50</v>
@@ -2267,12 +2311,12 @@
         <v>298.7124</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C103">
         <v>50</v>
@@ -2284,12 +2328,12 @@
         <v>328.44279999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C104">
         <v>50</v>
@@ -2307,45 +2351,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2357,12 +2401,12 @@
         <v>152.04099842511204</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2374,12 +2418,12 @@
         <v>181.92584578766815</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2391,12 +2435,12 @@
         <v>176.69000235439722</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2408,12 +2452,12 @@
         <v>163.96932904686614</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2425,12 +2469,12 @@
         <v>127.13557007002369</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2442,12 +2486,12 @@
         <v>93.243019878390101</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -2459,12 +2503,12 @@
         <v>67.73815858873273</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2476,12 +2520,12 @@
         <v>49.44101816325054</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2493,12 +2537,12 @@
         <v>40.858970665471325</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2510,12 +2554,12 @@
         <v>31.971859558155149</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2527,12 +2571,12 @@
         <v>24.661387296750803</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2544,12 +2588,12 @@
         <v>16.480927966595413</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2561,12 +2605,12 @@
         <v>10.856384678465073</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2578,12 +2622,12 @@
         <v>8.7482618594028025</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2595,12 +2639,12 @@
         <v>7.8551498604902301</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2612,12 +2656,12 @@
         <v>105.03801542729263</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2629,12 +2673,12 @@
         <v>57.945290836505293</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2646,12 +2690,12 @@
         <v>48.559894360281739</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2663,12 +2707,12 @@
         <v>29.297624593395174</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2680,12 +2724,12 @@
         <v>124.10847850026806</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2697,12 +2741,12 @@
         <v>157.52907981319805</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2714,12 +2758,12 @@
         <v>156.04341367876793</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2731,12 +2775,12 @@
         <v>153.23020648520202</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2748,12 +2792,12 @@
         <v>131.29674030988633</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2765,12 +2809,12 @@
         <v>115.02323460080564</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2782,12 +2826,12 @@
         <v>102.29331048974015</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2799,12 +2843,12 @@
         <v>74.13755471371806</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2816,12 +2860,12 @@
         <v>59.460551255625504</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2833,12 +2877,12 @@
         <v>45.35560544460381</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2850,12 +2894,12 @@
         <v>32.630109213485106</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2867,12 +2911,12 @@
         <v>18.941261939921056</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2884,12 +2928,12 @@
         <v>12.930862227366529</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2901,12 +2945,12 @@
         <v>11.079452137928971</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2918,12 +2962,12 @@
         <v>9.0505472238896854</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2935,12 +2979,12 @@
         <v>56.47546713925982</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2952,12 +2996,12 @@
         <v>32.404285948045633</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2969,12 +3013,12 @@
         <v>38.558842923372019</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2986,12 +3030,12 @@
         <v>49.269698530945874</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -3003,12 +3047,12 @@
         <v>179.59963873486504</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -3020,12 +3064,12 @@
         <v>220.06821865436271</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -3037,12 +3081,12 @@
         <v>203.02473003603984</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -3054,12 +3098,12 @@
         <v>194.92802021187975</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -3071,12 +3115,12 @@
         <v>174.26618403842591</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -3088,12 +3132,12 @@
         <v>161.40451003506172</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -3105,12 +3149,12 @@
         <v>158.37026692234406</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -3122,12 +3166,12 @@
         <v>123.78397132409022</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -3139,12 +3183,12 @@
         <v>112.61516609600189</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -3156,12 +3200,12 @@
         <v>93.176363717168158</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -3173,12 +3217,12 @@
         <v>75.483784561489259</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -3190,12 +3234,12 @@
         <v>55.160963299368959</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -3207,12 +3251,12 @@
         <v>37.237886001411169</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -3224,12 +3268,12 @@
         <v>32.974184632722711</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -3241,12 +3285,12 @@
         <v>22.035927698513191</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -3258,12 +3302,12 @@
         <v>109.99352690605313</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -3275,12 +3319,12 @@
         <v>86.025588612847869</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -3292,12 +3336,12 @@
         <v>101.58666576844553</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -3309,12 +3353,12 @@
         <v>104.40322657729121</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C59">
         <v>4</v>
@@ -3326,12 +3370,12 @@
         <v>183.24172428406899</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C60">
         <v>4</v>
@@ -3343,12 +3387,12 @@
         <v>213.41482884694602</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C61">
         <v>4</v>
@@ -3360,12 +3404,12 @@
         <v>202.9483765000391</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C62">
         <v>4</v>
@@ -3377,12 +3421,12 @@
         <v>197.30263163235151</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C63">
         <v>4</v>
@@ -3394,12 +3438,12 @@
         <v>185.7110851275097</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C64">
         <v>4</v>
@@ -3411,12 +3455,12 @@
         <v>176.95532398048354</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C65">
         <v>4</v>
@@ -3428,12 +3472,12 @@
         <v>175.12399373565361</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C66">
         <v>4</v>
@@ -3445,12 +3489,12 @@
         <v>152.26854822785583</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C67">
         <v>4</v>
@@ -3462,12 +3506,12 @@
         <v>151.86866913547345</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C68">
         <v>4</v>
@@ -3479,12 +3523,12 @@
         <v>142.39793435909462</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C69">
         <v>4</v>
@@ -3496,12 +3540,12 @@
         <v>133.769895978139</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C70">
         <v>4</v>
@@ -3513,12 +3557,12 @@
         <v>123.85839198014361</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C71">
         <v>4</v>
@@ -3530,12 +3574,12 @@
         <v>111.26301793312224</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C72">
         <v>4</v>
@@ -3547,12 +3591,12 @@
         <v>114.39840789155198</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C73">
         <v>4</v>
@@ -3564,12 +3608,12 @@
         <v>100.62993958440249</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C74">
         <v>4</v>
@@ -3581,12 +3625,12 @@
         <v>182.91787839510755</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C75">
         <v>4</v>
@@ -3598,12 +3642,12 @@
         <v>163.29050789869405</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C76">
         <v>4</v>
@@ -3615,12 +3659,12 @@
         <v>169.16600596140955</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C77">
         <v>4</v>
@@ -3632,12 +3676,12 @@
         <v>183.57835194243188</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C78">
         <v>8</v>
@@ -3649,12 +3693,12 @@
         <v>150.9633574239212</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C79">
         <v>8</v>
@@ -3666,12 +3710,12 @@
         <v>206.82338274807677</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C80">
         <v>8</v>
@@ -3683,12 +3727,12 @@
         <v>202.18956301504664</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C81">
         <v>8</v>
@@ -3700,12 +3744,12 @@
         <v>194.44541350961936</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C82">
         <v>8</v>
@@ -3717,12 +3761,12 @@
         <v>185.61501316610548</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C83">
         <v>8</v>
@@ -3734,12 +3778,12 @@
         <v>177.88907477707852</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C84">
         <v>8</v>
@@ -3751,12 +3795,12 @@
         <v>174.24283508262397</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C85">
         <v>8</v>
@@ -3768,12 +3812,12 @@
         <v>155.98919615896301</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B86" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C86">
         <v>8</v>
@@ -3785,12 +3829,12 @@
         <v>157.40732747866829</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C87">
         <v>8</v>
@@ -3802,12 +3846,12 @@
         <v>150.95610092130528</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C88">
         <v>8</v>
@@ -3819,12 +3863,12 @@
         <v>144.0145582918172</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C89">
         <v>8</v>
@@ -3836,12 +3880,12 @@
         <v>132.22259322942034</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C90">
         <v>8</v>
@@ -3853,12 +3897,12 @@
         <v>120.82006768879845</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C91">
         <v>8</v>
@@ -3870,12 +3914,12 @@
         <v>125.52786589806021</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C92">
         <v>8</v>
@@ -3887,12 +3931,12 @@
         <v>114.20166915133575</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B93" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C93">
         <v>8</v>
@@ -3904,12 +3948,12 @@
         <v>179.51477211419677</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C94">
         <v>8</v>
@@ -3921,12 +3965,12 @@
         <v>164.12707850195022</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C95">
         <v>8</v>
@@ -3938,12 +3982,12 @@
         <v>162.39594377941569</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C96">
         <v>8</v>
@@ -3955,12 +3999,12 @@
         <v>170.50909068764093</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B97" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C97">
         <v>16</v>
@@ -3972,12 +4016,12 @@
         <v>169.1216049230471</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B98" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C98">
         <v>16</v>
@@ -3989,12 +4033,12 @@
         <v>214.02576324202553</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C99">
         <v>16</v>
@@ -4006,12 +4050,12 @@
         <v>207.32411512671749</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C100">
         <v>16</v>
@@ -4023,12 +4067,12 @@
         <v>201.38598910184555</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C101">
         <v>16</v>
@@ -4040,12 +4084,12 @@
         <v>190.24124197542591</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C102">
         <v>16</v>
@@ -4057,12 +4101,12 @@
         <v>182.05100502274826</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C103">
         <v>16</v>
@@ -4074,12 +4118,12 @@
         <v>178.10118458547061</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C104">
         <v>16</v>
@@ -4091,12 +4135,12 @@
         <v>159.18166066273386</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C105">
         <v>16</v>
@@ -4108,12 +4152,12 @@
         <v>160.7055493854574</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C106">
         <v>16</v>
@@ -4125,12 +4169,12 @@
         <v>154.58721069920571</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C107">
         <v>16</v>
@@ -4142,12 +4186,12 @@
         <v>145.42408108761236</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B108" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C108">
         <v>16</v>
@@ -4159,12 +4203,12 @@
         <v>136.14882280764692</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B109" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C109">
         <v>16</v>
@@ -4176,12 +4220,12 @@
         <v>124.35177762821345</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B110" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C110">
         <v>16</v>
@@ -4193,12 +4237,12 @@
         <v>128.24191695158416</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B111" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C111">
         <v>16</v>
@@ -4210,12 +4254,12 @@
         <v>119.20029252668598</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B112" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C112">
         <v>16</v>
@@ -4227,12 +4271,12 @@
         <v>179.51477211419677</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B113" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C113">
         <v>16</v>
@@ -4244,12 +4288,12 @@
         <v>167.9532791004051</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B114" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C114">
         <v>16</v>
@@ -4261,12 +4305,12 @@
         <v>167.68370850270514</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C115">
         <v>16</v>
@@ -4284,31 +4328,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>35461</v>
@@ -4317,9 +4361,9 @@
         <v>12.121851647490036</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <f>EOMONTH(B2,1)</f>
@@ -4329,9 +4373,9 @@
         <v>12.343995306963409</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B30" si="0">EOMONTH(B3,1)</f>
@@ -4341,9 +4385,9 @@
         <v>12.735547597158529</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
@@ -4353,9 +4397,9 @@
         <v>9.1811987804487085</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
@@ -4365,9 +4409,9 @@
         <v>8.3687289803247573</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
@@ -4377,9 +4421,9 @@
         <v>8.0661618442851371</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
@@ -4389,9 +4433,9 @@
         <v>7.8189330258034841</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
@@ -4401,9 +4445,9 @@
         <v>8.2398489738840759</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
@@ -4413,9 +4457,9 @@
         <v>9.3340038721816398</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
@@ -4425,9 +4469,9 @@
         <v>10.289440196249025</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
@@ -4437,9 +4481,9 @@
         <v>10.382511301365486</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
@@ -4449,9 +4493,9 @@
         <v>10.29216312352051</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
@@ -4461,9 +4505,9 @@
         <v>14.165790954147262</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
@@ -4473,9 +4517,9 @@
         <v>14.14037244410795</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
@@ -4485,9 +4529,9 @@
         <v>12.323056210191114</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
@@ -4497,9 +4541,9 @@
         <v>11.155993708832277</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
@@ -4509,9 +4553,9 @@
         <v>8.7708675038193764</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
@@ -4521,9 +4565,9 @@
         <v>7.9416945244039461</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
@@ -4533,9 +4577,9 @@
         <v>7.3768208359985126</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
@@ -4545,9 +4589,9 @@
         <v>7.9603953268639405</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
@@ -4557,9 +4601,9 @@
         <v>8.7506212588492343</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
@@ -4569,9 +4613,9 @@
         <v>9.317809470879487</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
@@ -4581,9 +4625,9 @@
         <v>10.307153557247581</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
@@ -4593,9 +4637,9 @@
         <v>10.721326803922032</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
@@ -4605,9 +4649,9 @@
         <v>11.465810359771984</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
@@ -4617,9 +4661,9 @@
         <v>11.474705140019111</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
@@ -4629,9 +4673,9 @@
         <v>17.795044425792074</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
@@ -4641,9 +4685,9 @@
         <v>13.546130877463302</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
@@ -4659,39 +4703,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>35543</v>
@@ -4706,9 +4750,9 @@
         <v>2.7720045900732995</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>35577</v>
@@ -4723,9 +4767,9 @@
         <v>3.1376644178920317</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>35635</v>
@@ -4740,9 +4784,9 @@
         <v>3.861495219202812</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>35689</v>
@@ -4757,9 +4801,9 @@
         <v>4.4511819958988381</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>35759</v>
@@ -4774,9 +4818,9 @@
         <v>10.648302795031057</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>35822</v>
@@ -4791,9 +4835,9 @@
         <v>8.0183152238950726</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>35878</v>
@@ -4808,9 +4852,9 @@
         <v>11.113928409151749</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>35941</v>
@@ -4825,9 +4869,9 @@
         <v>12.826608487375578</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>36054</v>
@@ -4842,9 +4886,9 @@
         <v>11.077797403659533</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>36279</v>

</xml_diff>